<commit_message>
Project Files removed and added again
I removed the files from the directory and staging area then added again as there are some of the file which are being tracked by defaults, not following gitignore entries.
</commit_message>
<xml_diff>
--- a/temp/EXCEL/Steganography Results.xlsx
+++ b/temp/EXCEL/Steganography Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff1ba2c4b17edc7d/Documents/DIP Projects Others/Monika Sharma DIP Project/algo/proposed algo/temp/EXCEL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\F\Programming-in-XYZ\DIP\Project Jan 2022\proposed algo\temp\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{68FAEAAF-18FD-4D14-B3EE-BFC3A9D06C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED188884-B58F-415E-91D7-6CB7EE76C229}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A42511-B85F-49F5-B862-CB95993EAE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{50609699-6D32-4D2D-BAC0-1E434FB2C1AE}"/>
   </bookViews>

</xml_diff>

<commit_message>
Final commit after extra branch removd
Some unused branches are removed from both local and remote. Production is for major changes and Testing is more small changes.
</commit_message>
<xml_diff>
--- a/temp/EXCEL/Steganography Results.xlsx
+++ b/temp/EXCEL/Steganography Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff1ba2c4b17edc7d/Documents/DIP Projects Others/Monika Sharma DIP Project/algo/proposed algo/temp/EXCEL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\F\Programming-in-XYZ\DIP\Project Jan 2022\monika proposed algo\temp\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{68FAEAAF-18FD-4D14-B3EE-BFC3A9D06C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED188884-B58F-415E-91D7-6CB7EE76C229}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05CA531-2FF7-4723-BA5A-CF41EC57D0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{50609699-6D32-4D2D-BAC0-1E434FB2C1AE}"/>
   </bookViews>

</xml_diff>